<commit_message>
Client: Fix Can't Attack Bug
shift 누를때 펀치 안나가던 버그 고침
(원인) 기존 조작법에 해당하는 shift를 사용하는 애니메이션 자리를 만들어 놨는데 아무것도 안들어가 있었음
(해결) 현재 조작법에서는 제외하기로 했기 때문에 if문 삭제
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Ch_Stat.xlsx
+++ b/Server/Server/GameData/Ch_Stat.xlsx
@@ -57,7 +57,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   Value = 0 -&gt;  해당사항없음</t>
+  Value = 0 -&gt;  해당사항없음</t>
         </r>
       </text>
     </comment>
@@ -74,7 +74,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   공격속도</t>
+  공격속도</t>
         </r>
       </text>
     </comment>
@@ -91,7 +91,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   M로 계산</t>
+  M로 계산</t>
         </r>
       </text>
     </comment>
@@ -108,7 +108,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   스테미나 소모값
+  스테미나 소모값
 Ch_Hold는 초당으로 계산</t>
         </r>
       </text>
@@ -126,7 +126,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   공격 성공 시 상대방이 깍이는 스테미나</t>
+  공격 성공 시 상대방이 깍이는 스테미나</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   Value = 0 이면 해당사항 없음</t>
+  Value = 0 이면 해당사항 없음</t>
         </r>
       </text>
     </comment>
@@ -170,7 +170,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   초당으로 계산
+  초당으로 계산
 Ch_Dash는 횟수로 계산</t>
         </r>
       </text>
@@ -198,7 +198,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   행동속도 (초로 계산)</t>
+  행동속도 (초로 계산)</t>
         </r>
       </text>
     </comment>
@@ -215,7 +215,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   오브젝트와 거리 
+  오브젝트와 거리 
 원 모양
 반지름으로 계산
 M로 계산</t>
@@ -235,7 +235,7 @@
           <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-   스테미나 소모값
+  스테미나 소모값
 Ch_Hold는 초당으로 계산</t>
         </r>
       </text>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1180,7 +1180,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0.60</v>
+        <v>0.50</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1.20</v>
+        <v>0.80</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1231,7 +1231,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>1.80</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1265,7 +1265,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>0.90</v>
+        <v>0.70</v>
       </c>
       <c r="D8">
         <v>5</v>

</xml_diff>

<commit_message>
Server: disconnect한 player delete 시 오류 수정
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Ch_Stat.xlsx
+++ b/Server/Server/GameData/Ch_Stat.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\FestivalTownProject\Client\Assets\11. GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F0A4C6-28C5-4B58-8EF0-CC736E61E759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25605" yWindow="3165" windowWidth="22680" windowHeight="11295" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Stat" sheetId="2" r:id="rId4"/>
-    <sheet name="Attack" sheetId="1" r:id="rId5"/>
-    <sheet name="Move" sheetId="3" r:id="rId6"/>
-    <sheet name="Action" sheetId="5" r:id="rId7"/>
+    <sheet name="Stat" sheetId="2" r:id="rId1"/>
+    <sheet name="Attack" sheetId="1" r:id="rId2"/>
+    <sheet name="Move" sheetId="3" r:id="rId3"/>
+    <sheet name="Action" sheetId="5" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,13 +38,13 @@
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>김혁동(2017180008)</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -134,13 +134,13 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>김혁동(2017180008)</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -179,13 +179,13 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>김혁동(2017180008)</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -202,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -347,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,12 +355,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -377,6 +371,13 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -402,119 +403,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+  <cellStyles count="1">
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -527,9 +436,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="경천 강" id="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" userId="9a4f2fb646cdd437" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -848,26 +755,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F961BFE-AEF0-4053-AE30-EADB432CB913}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F961BFE-AEF0-4053-AE30-EADB432CB913}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -887,7 +794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -908,30 +815,31 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB07990-B5DE-4DA3-A25A-FCE377F249C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB07990-B5DE-4DA3-A25A-FCE377F249C7}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -954,7 +862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -962,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -977,7 +885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -985,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1.30</v>
+        <v>1.3</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1.30</v>
+        <v>1.3</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -1000,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10003</v>
       </c>
@@ -1014,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1.40</v>
+        <v>1.4</v>
       </c>
       <c r="F4">
         <v>15</v>
@@ -1023,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10004</v>
       </c>
@@ -1046,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>10005</v>
       </c>
@@ -1069,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>10006</v>
       </c>
@@ -1077,13 +985,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.80</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.30</v>
+        <v>0.3</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -1092,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>10007</v>
       </c>
@@ -1116,29 +1024,30 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C159E774-2D2E-4E42-A34F-C2E138094600}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C159E774-2D2E-4E42-A34F-C2E138094600}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>20001</v>
       </c>
@@ -1172,7 +1081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>20002</v>
       </c>
@@ -1180,7 +1089,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0.50</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1189,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>20003</v>
       </c>
@@ -1197,7 +1106,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0.80</v>
+        <v>1.3</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1206,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>20004</v>
       </c>
@@ -1223,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>20005</v>
       </c>
@@ -1240,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>20006</v>
       </c>
@@ -1248,7 +1157,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>0.40</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1257,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>20007</v>
       </c>
@@ -1265,7 +1174,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>0.70</v>
+        <v>0.7</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1274,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>20008</v>
       </c>
@@ -1292,28 +1201,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E578D4C-D8A7-4CED-8428-0F9C08F4A41C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E578D4C-D8A7-4CED-8428-0F9C08F4A41C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1330,7 +1240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>30001</v>
       </c>
@@ -1338,7 +1248,7 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1347,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>30002</v>
       </c>
@@ -1355,7 +1265,7 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>0.50</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1365,7 +1275,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Client: Fix Weapon Delete Bug
무기 들고 떨어졌을때 서버 터지는 문제 해결
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Ch_Stat.xlsx
+++ b/Server/Server/GameData/Ch_Stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F0A4C6-28C5-4B58-8EF0-CC736E61E759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18280C7A-6AD2-4B22-AEA3-2E7B11A5D9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,10 +433,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1035,7 +1031,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1157,7 +1153,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1174,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>5</v>

</xml_diff>